<commit_message>
Fixing issues with analysis templates
</commit_message>
<xml_diff>
--- a/src/assets/empty/faang_analysis.xlsx
+++ b/src/assets/empty/faang_analysis.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/empty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47321D58-1F41-1541-A5FB-770571A07FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477660ED-58B4-F94B-8AD5-21BD81793990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="500" windowWidth="27640" windowHeight="16040" xr2:uid="{D8AC673E-FE7C-174A-B15F-CD4D6641A206}"/>
+    <workbookView xWindow="40000" yWindow="2160" windowWidth="27640" windowHeight="16040" activeTab="1" xr2:uid="{D8AC673E-FE7C-174A-B15F-CD4D6641A206}"/>
   </bookViews>
   <sheets>
-    <sheet name="faang" sheetId="1" r:id="rId1"/>
-    <sheet name="ena" sheetId="2" r:id="rId2"/>
-    <sheet name="eva" sheetId="3" r:id="rId3"/>
-    <sheet name="faang_field_values" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="submission" sheetId="5" r:id="rId1"/>
+    <sheet name="faang" sheetId="1" r:id="rId2"/>
+    <sheet name="ena" sheetId="2" r:id="rId3"/>
+    <sheet name="eva" sheetId="3" r:id="rId4"/>
+    <sheet name="faang_field_values" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="145">
   <si>
     <t>Alias</t>
   </si>
@@ -468,7 +469,7 @@
     <t>Illumina MiSeq</t>
   </si>
   <si>
-    <t>Analysis Version</t>
+    <t>Analysis Code Version</t>
   </si>
 </sst>
 </file>
@@ -902,22 +903,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1297745-C72E-E14C-A733-549001216631}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3FCF971-7D08-D749-9B35-64EAEF14B736}">
   <dimension ref="A1:H201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="101.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1737,7 +1756,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52862032-400E-D045-982F-14567BAC1D37}">
   <dimension ref="A1:S201"/>
   <sheetViews>
@@ -4093,7 +4112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF121EC-CD54-D140-8952-93B4B3FE79C0}">
   <dimension ref="A1:W1"/>
   <sheetViews>
@@ -4219,7 +4238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5136D478-A861-6B4B-92CD-33DFA810AC18}">
   <dimension ref="A1:AX7"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated spreadsheet examples for analyses (assets folder)
</commit_message>
<xml_diff>
--- a/src/assets/empty/faang_analysis.xlsx
+++ b/src/assets/empty/faang_analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexey/ebi_projects/faang-portal-frontend/src/assets/empty/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yroochun/Projects/dcc-portal-frontend/src/assets/empty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477660ED-58B4-F94B-8AD5-21BD81793990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212FCE15-8DC0-2C4A-9776-D3D74D2EAD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40000" yWindow="2160" windowWidth="27640" windowHeight="16040" activeTab="1" xr2:uid="{D8AC673E-FE7C-174A-B15F-CD4D6641A206}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="147">
   <si>
     <t>Alias</t>
   </si>
@@ -470,6 +470,12 @@
   </si>
   <si>
     <t>Analysis Code Version</t>
+  </si>
+  <si>
+    <t>Nextflow Config Url</t>
+  </si>
+  <si>
+    <t>Nextflow Spreadsheet Url</t>
   </si>
 </sst>
 </file>
@@ -922,10 +928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3FCF971-7D08-D749-9B35-64EAEF14B736}">
-  <dimension ref="A1:H201"/>
+  <dimension ref="A1:J201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -938,9 +944,11 @@
     <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -965,64 +973,70 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="E16" s="3"/>
     </row>

</xml_diff>